<commit_message>
JinL - change "graduate" level to "master 3" for 3 students
</commit_message>
<xml_diff>
--- a/data-transfer/transfer/data/calphi/student.xlsx
+++ b/data-transfer/transfer/data/calphi/student.xlsx
@@ -608,9 +608,6 @@
     <t>Raina Mandayam</t>
   </si>
   <si>
-    <t>Graduate</t>
-  </si>
-  <si>
     <t>650-207-3612</t>
   </si>
   <si>
@@ -1329,6 +1326,9 @@
   </si>
   <si>
     <t>9/1/2016</t>
+  </si>
+  <si>
+    <t>Master 3</t>
   </si>
 </sst>
 </file>
@@ -1830,9 +1830,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X353"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
       <pane xSplit="4" topLeftCell="E1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="Q44" sqref="Q44"/>
+      <selection pane="topRight" activeCell="F46" sqref="F46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1937,7 +1937,7 @@
         <v>24</v>
       </c>
       <c r="F2" s="33" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="G2" s="11" t="s">
         <v>25</v>
@@ -1964,7 +1964,7 @@
         <v>23</v>
       </c>
       <c r="Q2" s="33" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="R2" s="16">
         <v>0.39583333333333331</v>
@@ -1973,7 +1973,7 @@
         <v>31</v>
       </c>
       <c r="U2" s="35" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="3" spans="1:24" s="11" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1991,7 +1991,7 @@
         <v>24</v>
       </c>
       <c r="F3" s="33" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="G3" s="11" t="s">
         <v>34</v>
@@ -2018,7 +2018,7 @@
         <v>37</v>
       </c>
       <c r="Q3" s="33" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="R3" s="16">
         <v>0.40625</v>
@@ -2027,7 +2027,7 @@
         <v>31</v>
       </c>
       <c r="U3" s="35" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="4" spans="1:24" s="11" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2045,7 +2045,7 @@
         <v>39</v>
       </c>
       <c r="F4" s="33" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="G4" s="14" t="s">
         <v>40</v>
@@ -2072,7 +2072,7 @@
         <v>37</v>
       </c>
       <c r="Q4" s="33" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="R4" s="16">
         <v>0.40625</v>
@@ -2081,7 +2081,7 @@
         <v>31</v>
       </c>
       <c r="U4" s="35" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="W4" s="11" t="str">
         <f t="shared" ref="W4:W67" si="0">CONCATENATE(L4,M4,N4,O4,Q4)</f>
@@ -2107,7 +2107,7 @@
         <v>24</v>
       </c>
       <c r="F5" s="33" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="G5" s="14" t="s">
         <v>44</v>
@@ -2134,7 +2134,7 @@
         <v>47</v>
       </c>
       <c r="Q5" s="33" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="R5" s="16">
         <v>0.40625</v>
@@ -2143,7 +2143,7 @@
         <v>31</v>
       </c>
       <c r="U5" s="35" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="W5" s="11" t="str">
         <f t="shared" si="0"/>
@@ -2169,7 +2169,7 @@
         <v>24</v>
       </c>
       <c r="F6" s="33" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="G6" s="14" t="s">
         <v>49</v>
@@ -2196,7 +2196,7 @@
         <v>47</v>
       </c>
       <c r="Q6" s="33" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="R6" s="16">
         <v>0.40625</v>
@@ -2205,7 +2205,7 @@
         <v>31</v>
       </c>
       <c r="U6" s="35" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="W6" s="11" t="str">
         <f t="shared" si="0"/>
@@ -2231,7 +2231,7 @@
         <v>24</v>
       </c>
       <c r="F7" s="33" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="G7" s="19" t="s">
         <v>49</v>
@@ -2258,7 +2258,7 @@
         <v>47</v>
       </c>
       <c r="Q7" s="33" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="R7" s="16">
         <v>0.40625</v>
@@ -2267,7 +2267,7 @@
         <v>31</v>
       </c>
       <c r="U7" s="35" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="W7" s="11" t="str">
         <f t="shared" si="0"/>
@@ -2293,7 +2293,7 @@
         <v>39</v>
       </c>
       <c r="F8" s="33" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="G8" s="20" t="s">
         <v>54</v>
@@ -2320,7 +2320,7 @@
         <v>47</v>
       </c>
       <c r="Q8" s="33" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="R8" s="16">
         <v>0.40625</v>
@@ -2329,7 +2329,7 @@
         <v>31</v>
       </c>
       <c r="U8" s="35" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="W8" s="11" t="str">
         <f t="shared" si="0"/>
@@ -2355,7 +2355,7 @@
         <v>39</v>
       </c>
       <c r="F9" s="33" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="G9" s="11" t="s">
         <v>34</v>
@@ -2382,7 +2382,7 @@
         <v>59</v>
       </c>
       <c r="Q9" s="33" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="R9" s="16">
         <v>0.41666666666666669</v>
@@ -2391,7 +2391,7 @@
         <v>31</v>
       </c>
       <c r="U9" s="35" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="W9" s="11" t="str">
         <f t="shared" si="0"/>
@@ -2417,7 +2417,7 @@
         <v>39</v>
       </c>
       <c r="F10" s="33" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="G10" s="14" t="s">
         <v>40</v>
@@ -2444,7 +2444,7 @@
         <v>59</v>
       </c>
       <c r="Q10" s="33" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="R10" s="16">
         <v>0.41666666666666669</v>
@@ -2453,7 +2453,7 @@
         <v>31</v>
       </c>
       <c r="U10" s="35" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="W10" s="11" t="str">
         <f t="shared" si="0"/>
@@ -2479,7 +2479,7 @@
         <v>24</v>
       </c>
       <c r="F11" s="33" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="G11" s="14" t="s">
         <v>63</v>
@@ -2506,7 +2506,7 @@
         <v>59</v>
       </c>
       <c r="Q11" s="33" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="R11" s="16">
         <v>0.41666666666666669</v>
@@ -2516,7 +2516,7 @@
       </c>
       <c r="T11" s="22"/>
       <c r="U11" s="36" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="W11" s="11" t="str">
         <f t="shared" si="0"/>
@@ -2542,7 +2542,7 @@
         <v>24</v>
       </c>
       <c r="F12" s="33" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="G12" s="14" t="s">
         <v>67</v>
@@ -2569,7 +2569,7 @@
         <v>69</v>
       </c>
       <c r="Q12" s="33" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="R12" s="16">
         <v>0.41666666666666669</v>
@@ -2579,7 +2579,7 @@
       </c>
       <c r="T12" s="22"/>
       <c r="U12" s="36" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="W12" s="11" t="str">
         <f t="shared" si="0"/>
@@ -2605,7 +2605,7 @@
         <v>24</v>
       </c>
       <c r="F13" s="33" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="G13" s="14" t="s">
         <v>72</v>
@@ -2632,7 +2632,7 @@
         <v>71</v>
       </c>
       <c r="Q13" s="33" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="R13" s="16">
         <v>0.4375</v>
@@ -2642,7 +2642,7 @@
       </c>
       <c r="T13" s="22"/>
       <c r="U13" s="36" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="W13" s="11" t="str">
         <f t="shared" si="0"/>
@@ -2668,7 +2668,7 @@
         <v>24</v>
       </c>
       <c r="F14" s="33" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="G14" s="14">
         <v>5105790135</v>
@@ -2695,7 +2695,7 @@
         <v>71</v>
       </c>
       <c r="Q14" s="33" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="R14" s="16">
         <v>0.4375</v>
@@ -2704,7 +2704,7 @@
         <v>31</v>
       </c>
       <c r="U14" s="35" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="W14" s="11" t="str">
         <f t="shared" si="0"/>
@@ -2730,7 +2730,7 @@
         <v>39</v>
       </c>
       <c r="F15" s="33" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="G15" s="14" t="s">
         <v>77</v>
@@ -2757,7 +2757,7 @@
         <v>37</v>
       </c>
       <c r="Q15" s="33" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="R15" s="16">
         <v>0.4375</v>
@@ -2766,7 +2766,7 @@
         <v>31</v>
       </c>
       <c r="U15" s="35" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="W15" s="11" t="str">
         <f t="shared" si="0"/>
@@ -2792,7 +2792,7 @@
         <v>24</v>
       </c>
       <c r="F16" s="33" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="G16" s="14" t="s">
         <v>72</v>
@@ -2819,7 +2819,7 @@
         <v>80</v>
       </c>
       <c r="Q16" s="33" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="R16" s="16">
         <v>0.4375</v>
@@ -2828,7 +2828,7 @@
         <v>31</v>
       </c>
       <c r="U16" s="35" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="W16" s="11" t="str">
         <f t="shared" si="0"/>
@@ -2854,7 +2854,7 @@
         <v>24</v>
       </c>
       <c r="F17" s="33" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="G17" s="14">
         <v>5105790135</v>
@@ -2881,7 +2881,7 @@
         <v>23</v>
       </c>
       <c r="Q17" s="33" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="R17" s="16">
         <v>0.4375</v>
@@ -2890,7 +2890,7 @@
         <v>31</v>
       </c>
       <c r="U17" s="35" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="W17" s="11" t="str">
         <f t="shared" si="0"/>
@@ -2912,7 +2912,7 @@
         <v>24</v>
       </c>
       <c r="F18" s="33" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="G18" s="14">
         <v>5105790135</v>
@@ -2939,7 +2939,7 @@
         <v>23</v>
       </c>
       <c r="Q18" s="34" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="R18" s="16">
         <v>0.4375</v>
@@ -2948,7 +2948,7 @@
         <v>31</v>
       </c>
       <c r="U18" s="35" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="W18" s="11" t="str">
         <f t="shared" si="0"/>
@@ -2974,7 +2974,7 @@
         <v>24</v>
       </c>
       <c r="F19" s="33" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="G19" s="14">
         <v>4153779590</v>
@@ -3001,7 +3001,7 @@
         <v>23</v>
       </c>
       <c r="Q19" s="34" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="R19" s="16">
         <v>0.45833333333333331</v>
@@ -3010,7 +3010,7 @@
         <v>31</v>
       </c>
       <c r="U19" s="35" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="W19" s="11" t="str">
         <f t="shared" si="0"/>
@@ -3036,7 +3036,7 @@
         <v>24</v>
       </c>
       <c r="F20" s="33" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="G20" s="14">
         <v>5104291608</v>
@@ -3063,7 +3063,7 @@
         <v>71</v>
       </c>
       <c r="Q20" s="34" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="R20" s="16">
         <v>0.46875</v>
@@ -3072,7 +3072,7 @@
         <v>31</v>
       </c>
       <c r="U20" s="35" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="W20" s="11" t="str">
         <f t="shared" si="0"/>
@@ -3098,7 +3098,7 @@
         <v>39</v>
       </c>
       <c r="F21" s="33" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="G21" s="14">
         <v>5104291608</v>
@@ -3125,7 +3125,7 @@
         <v>37</v>
       </c>
       <c r="Q21" s="34" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="R21" s="16">
         <v>0.46875</v>
@@ -3135,7 +3135,7 @@
       </c>
       <c r="T21" s="24"/>
       <c r="U21" s="37" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="W21" s="11" t="str">
         <f t="shared" si="0"/>
@@ -3161,7 +3161,7 @@
         <v>39</v>
       </c>
       <c r="F22" s="33" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="G22" s="14" t="s">
         <v>90</v>
@@ -3188,7 +3188,7 @@
         <v>80</v>
       </c>
       <c r="Q22" s="34" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="R22" s="16">
         <v>0.46875</v>
@@ -3198,7 +3198,7 @@
       </c>
       <c r="T22" s="22"/>
       <c r="U22" s="36" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="W22" s="11" t="str">
         <f t="shared" si="0"/>
@@ -3224,7 +3224,7 @@
         <v>24</v>
       </c>
       <c r="F23" s="33" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="G23" s="14" t="s">
         <v>94</v>
@@ -3251,7 +3251,7 @@
         <v>59</v>
       </c>
       <c r="Q23" s="34" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="R23" s="16">
         <v>0.45833333333333331</v>
@@ -3261,7 +3261,7 @@
       </c>
       <c r="T23" s="22"/>
       <c r="U23" s="36" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="W23" s="11" t="str">
         <f t="shared" si="0"/>
@@ -3287,7 +3287,7 @@
         <v>39</v>
       </c>
       <c r="F24" s="35" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="G24" s="14" t="s">
         <v>98</v>
@@ -3314,7 +3314,7 @@
         <v>59</v>
       </c>
       <c r="Q24" s="34" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="R24" s="16">
         <v>0.45833333333333331</v>
@@ -3324,7 +3324,7 @@
       </c>
       <c r="T24" s="22"/>
       <c r="U24" s="36" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="W24" s="11" t="str">
         <f t="shared" si="0"/>
@@ -3350,7 +3350,7 @@
         <v>24</v>
       </c>
       <c r="F25" s="33" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="G25" s="14" t="s">
         <v>102</v>
@@ -3377,7 +3377,7 @@
         <v>104</v>
       </c>
       <c r="Q25" s="34" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="R25" s="16">
         <v>0.45833333333333331</v>
@@ -3387,7 +3387,7 @@
       </c>
       <c r="T25" s="22"/>
       <c r="U25" s="36" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="W25" s="11" t="str">
         <f t="shared" si="0"/>
@@ -3413,7 +3413,7 @@
         <v>39</v>
       </c>
       <c r="F26" s="33" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="G26" s="14" t="s">
         <v>107</v>
@@ -3440,7 +3440,7 @@
         <v>104</v>
       </c>
       <c r="Q26" s="34" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="R26" s="16">
         <v>0.45833333333333331</v>
@@ -3450,7 +3450,7 @@
       </c>
       <c r="T26" s="22"/>
       <c r="U26" s="36" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="W26" s="11" t="str">
         <f t="shared" si="0"/>
@@ -3476,7 +3476,7 @@
         <v>24</v>
       </c>
       <c r="F27" s="33" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="G27" s="14">
         <v>5104888100</v>
@@ -3503,7 +3503,7 @@
         <v>112</v>
       </c>
       <c r="Q27" s="34" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="R27" s="16">
         <v>0.47916666666666669</v>
@@ -3513,7 +3513,7 @@
       </c>
       <c r="T27" s="22"/>
       <c r="U27" s="36" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="W27" s="11" t="str">
         <f t="shared" si="0"/>
@@ -3539,7 +3539,7 @@
         <v>39</v>
       </c>
       <c r="F28" s="35" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="G28" s="14">
         <v>5104888100</v>
@@ -3566,7 +3566,7 @@
         <v>112</v>
       </c>
       <c r="Q28" s="34" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="R28" s="16">
         <v>0.47916666666666669</v>
@@ -3576,7 +3576,7 @@
       </c>
       <c r="T28" s="22"/>
       <c r="U28" s="36" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="W28" s="11" t="str">
         <f t="shared" si="0"/>
@@ -3602,7 +3602,7 @@
         <v>24</v>
       </c>
       <c r="F29" s="35" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="G29" s="14" t="s">
         <v>115</v>
@@ -3629,7 +3629,7 @@
         <v>37</v>
       </c>
       <c r="Q29" s="34" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="R29" s="16">
         <v>0.5</v>
@@ -3639,7 +3639,7 @@
       </c>
       <c r="T29" s="22"/>
       <c r="U29" s="36" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="W29" s="11" t="str">
         <f t="shared" si="0"/>
@@ -3665,7 +3665,7 @@
         <v>24</v>
       </c>
       <c r="F30" s="33" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="G30" s="14" t="s">
         <v>115</v>
@@ -3692,7 +3692,7 @@
         <v>59</v>
       </c>
       <c r="Q30" s="34" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="R30" s="16">
         <v>0.5</v>
@@ -3701,7 +3701,7 @@
         <v>31</v>
       </c>
       <c r="U30" s="35" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="W30" s="11" t="str">
         <f t="shared" si="0"/>
@@ -3727,7 +3727,7 @@
         <v>39</v>
       </c>
       <c r="F31" s="33" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="G31" s="11" t="s">
         <v>120</v>
@@ -3754,7 +3754,7 @@
         <v>23</v>
       </c>
       <c r="Q31" s="34" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="R31" s="16">
         <v>0.60416666666666663</v>
@@ -3763,7 +3763,7 @@
         <v>31</v>
       </c>
       <c r="U31" s="35" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="W31" s="11" t="str">
         <f t="shared" si="0"/>
@@ -3789,7 +3789,7 @@
         <v>24</v>
       </c>
       <c r="F32" s="33" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="G32" s="11" t="s">
         <v>120</v>
@@ -3816,7 +3816,7 @@
         <v>23</v>
       </c>
       <c r="Q32" s="34" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="R32" s="16">
         <v>0.60416666666666663</v>
@@ -3825,7 +3825,7 @@
         <v>31</v>
       </c>
       <c r="U32" s="35" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="W32" s="11" t="str">
         <f t="shared" si="0"/>
@@ -3851,7 +3851,7 @@
         <v>24</v>
       </c>
       <c r="F33" s="33" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="G33" s="11" t="s">
         <v>120</v>
@@ -3878,7 +3878,7 @@
         <v>23</v>
       </c>
       <c r="Q33" s="34" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="R33" s="16">
         <v>0.60416666666666663</v>
@@ -3887,7 +3887,7 @@
         <v>31</v>
       </c>
       <c r="U33" s="35" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="W33" s="11" t="str">
         <f t="shared" si="0"/>
@@ -3913,7 +3913,7 @@
         <v>24</v>
       </c>
       <c r="F34" s="33" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="G34" s="14" t="s">
         <v>125</v>
@@ -3940,7 +3940,7 @@
         <v>112</v>
       </c>
       <c r="Q34" s="34" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="R34" s="16">
         <v>0.60416666666666663</v>
@@ -3949,7 +3949,7 @@
         <v>31</v>
       </c>
       <c r="U34" s="35" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="W34" s="11" t="str">
         <f t="shared" si="0"/>
@@ -3975,7 +3975,7 @@
         <v>39</v>
       </c>
       <c r="F35" s="33" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="G35" s="14">
         <v>5103326113</v>
@@ -4002,7 +4002,7 @@
         <v>112</v>
       </c>
       <c r="Q35" s="34" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="R35" s="16">
         <v>0.60416666666666663</v>
@@ -4011,7 +4011,7 @@
         <v>31</v>
       </c>
       <c r="U35" s="35" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="W35" s="11" t="str">
         <f t="shared" si="0"/>
@@ -4037,7 +4037,7 @@
         <v>24</v>
       </c>
       <c r="F36" s="33" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="G36" s="14" t="s">
         <v>131</v>
@@ -4064,7 +4064,7 @@
         <v>112</v>
       </c>
       <c r="Q36" s="34" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="R36" s="16">
         <v>0.60416666666666663</v>
@@ -4073,7 +4073,7 @@
         <v>31</v>
       </c>
       <c r="U36" s="35" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="W36" s="11" t="str">
         <f t="shared" si="0"/>
@@ -4099,7 +4099,7 @@
         <v>24</v>
       </c>
       <c r="F37" s="35" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="G37" s="14">
         <v>4085987667</v>
@@ -4126,7 +4126,7 @@
         <v>23</v>
       </c>
       <c r="Q37" s="34" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="R37" s="16">
         <v>0.625</v>
@@ -4136,7 +4136,7 @@
       </c>
       <c r="T37" s="22"/>
       <c r="U37" s="36" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="W37" s="11" t="str">
         <f t="shared" si="0"/>
@@ -4162,7 +4162,7 @@
         <v>39</v>
       </c>
       <c r="F38" s="33" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="G38" s="14">
         <v>4085987366</v>
@@ -4189,7 +4189,7 @@
         <v>112</v>
       </c>
       <c r="Q38" s="34" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="R38" s="16">
         <v>0.625</v>
@@ -4198,7 +4198,7 @@
         <v>31</v>
       </c>
       <c r="U38" s="35" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="W38" s="11" t="str">
         <f t="shared" si="0"/>
@@ -4224,7 +4224,7 @@
         <v>39</v>
       </c>
       <c r="F39" s="35" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="G39" s="14" t="s">
         <v>125</v>
@@ -4251,7 +4251,7 @@
         <v>80</v>
       </c>
       <c r="Q39" s="34" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="R39" s="16">
         <v>0.61458333333333337</v>
@@ -4260,7 +4260,7 @@
         <v>31</v>
       </c>
       <c r="U39" s="35" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="W39" s="11" t="str">
         <f t="shared" si="0"/>
@@ -4286,7 +4286,7 @@
         <v>39</v>
       </c>
       <c r="F40" s="33" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="G40" s="14" t="s">
         <v>138</v>
@@ -4313,7 +4313,7 @@
         <v>80</v>
       </c>
       <c r="Q40" s="34" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="R40" s="16">
         <v>0.61458333333333337</v>
@@ -4322,7 +4322,7 @@
         <v>31</v>
       </c>
       <c r="U40" s="35" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="W40" s="11" t="str">
         <f t="shared" si="0"/>
@@ -4348,7 +4348,7 @@
         <v>24</v>
       </c>
       <c r="F41" s="35" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="G41" s="14">
         <v>6502089689</v>
@@ -4375,7 +4375,7 @@
         <v>47</v>
       </c>
       <c r="Q41" s="34" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="R41" s="16">
         <v>0.61458333333333337</v>
@@ -4384,7 +4384,7 @@
         <v>31</v>
       </c>
       <c r="U41" s="35" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="W41" s="11" t="str">
         <f t="shared" si="0"/>
@@ -4410,7 +4410,7 @@
         <v>39</v>
       </c>
       <c r="F42" s="35" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="G42" s="14" t="s">
         <v>143</v>
@@ -4437,7 +4437,7 @@
         <v>47</v>
       </c>
       <c r="Q42" s="34" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="R42" s="16">
         <v>0.61458333333333337</v>
@@ -4446,7 +4446,7 @@
         <v>31</v>
       </c>
       <c r="U42" s="35" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="W42" s="11" t="str">
         <f t="shared" si="0"/>
@@ -4472,7 +4472,7 @@
         <v>39</v>
       </c>
       <c r="F43" s="33" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="G43" s="14" t="s">
         <v>146</v>
@@ -4499,7 +4499,7 @@
         <v>59</v>
       </c>
       <c r="Q43" s="34" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="R43" s="16">
         <v>0.625</v>
@@ -4508,7 +4508,7 @@
         <v>31</v>
       </c>
       <c r="U43" s="35" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="W43" s="11" t="str">
         <f t="shared" si="0"/>
@@ -4534,7 +4534,7 @@
         <v>24</v>
       </c>
       <c r="F44" s="35" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="G44" s="14" t="s">
         <v>146</v>
@@ -4561,7 +4561,7 @@
         <v>59</v>
       </c>
       <c r="Q44" s="34" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="R44" s="16">
         <v>0.625</v>
@@ -4570,7 +4570,7 @@
         <v>31</v>
       </c>
       <c r="U44" s="35" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="W44" s="11" t="str">
         <f t="shared" si="0"/>
@@ -4596,7 +4596,7 @@
         <v>24</v>
       </c>
       <c r="F45" s="33" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="G45" s="26" t="s">
         <v>150</v>
@@ -4623,7 +4623,7 @@
         <v>59</v>
       </c>
       <c r="Q45" s="34" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="R45" s="16">
         <v>0.625</v>
@@ -4632,7 +4632,7 @@
         <v>31</v>
       </c>
       <c r="U45" s="35" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="W45" s="11" t="str">
         <f t="shared" si="0"/>
@@ -4658,7 +4658,7 @@
         <v>39</v>
       </c>
       <c r="F46" s="33" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G46" s="14" t="s">
         <v>153</v>
@@ -4685,7 +4685,7 @@
         <v>59</v>
       </c>
       <c r="Q46" s="34" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="R46" s="16">
         <v>0.625</v>
@@ -4695,7 +4695,7 @@
       </c>
       <c r="T46" s="22"/>
       <c r="U46" s="36" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="W46" s="11" t="str">
         <f t="shared" si="0"/>
@@ -4721,7 +4721,7 @@
         <v>24</v>
       </c>
       <c r="F47" s="33" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="G47" s="14" t="s">
         <v>155</v>
@@ -4746,7 +4746,7 @@
         <v>71</v>
       </c>
       <c r="Q47" s="34" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="R47" s="16">
         <v>0.64583333333333337</v>
@@ -4756,7 +4756,7 @@
       </c>
       <c r="T47" s="22"/>
       <c r="U47" s="36" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="W47" s="11" t="str">
         <f t="shared" si="0"/>
@@ -4782,7 +4782,7 @@
         <v>39</v>
       </c>
       <c r="F48" s="33" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="G48" s="14" t="s">
         <v>157</v>
@@ -4809,7 +4809,7 @@
         <v>71</v>
       </c>
       <c r="Q48" s="34" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="R48" s="16">
         <v>0.64583333333333337</v>
@@ -4819,7 +4819,7 @@
       </c>
       <c r="T48" s="22"/>
       <c r="U48" s="36" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="W48" s="11" t="str">
         <f t="shared" si="0"/>
@@ -4845,7 +4845,7 @@
         <v>39</v>
       </c>
       <c r="F49" s="33" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="G49" s="14" t="s">
         <v>157</v>
@@ -4872,7 +4872,7 @@
         <v>71</v>
       </c>
       <c r="Q49" s="34" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="R49" s="16">
         <v>0.64583333333333337</v>
@@ -4882,7 +4882,7 @@
       </c>
       <c r="T49" s="22"/>
       <c r="U49" s="36" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="W49" s="11" t="str">
         <f t="shared" si="0"/>
@@ -4908,7 +4908,7 @@
         <v>39</v>
       </c>
       <c r="F50" s="33" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="G50" s="14" t="s">
         <v>162</v>
@@ -4935,7 +4935,7 @@
         <v>37</v>
       </c>
       <c r="Q50" s="34" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="R50" s="16">
         <v>0.64583333333333337</v>
@@ -4945,7 +4945,7 @@
       </c>
       <c r="T50" s="22"/>
       <c r="U50" s="36" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="W50" s="11" t="str">
         <f t="shared" si="0"/>
@@ -4971,7 +4971,7 @@
         <v>24</v>
       </c>
       <c r="F51" s="33" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="G51" s="14" t="s">
         <v>162</v>
@@ -4998,7 +4998,7 @@
         <v>37</v>
       </c>
       <c r="Q51" s="34" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="R51" s="16">
         <v>0.64583333333333337</v>
@@ -5008,7 +5008,7 @@
       </c>
       <c r="T51" s="22"/>
       <c r="U51" s="36" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="W51" s="11" t="str">
         <f t="shared" si="0"/>
@@ -5034,7 +5034,7 @@
         <v>39</v>
       </c>
       <c r="F52" s="33" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="G52" s="14" t="s">
         <v>166</v>
@@ -5061,7 +5061,7 @@
         <v>47</v>
       </c>
       <c r="Q52" s="34" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="R52" s="16">
         <v>0.64583333333333337</v>
@@ -5071,7 +5071,7 @@
       </c>
       <c r="T52" s="22"/>
       <c r="U52" s="36" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="W52" s="11" t="str">
         <f t="shared" si="0"/>
@@ -5097,7 +5097,7 @@
         <v>39</v>
       </c>
       <c r="F53" s="33" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="G53" s="14" t="s">
         <v>131</v>
@@ -5124,7 +5124,7 @@
         <v>80</v>
       </c>
       <c r="Q53" s="34" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="R53" s="16">
         <v>0.64583333333333337</v>
@@ -5134,7 +5134,7 @@
       </c>
       <c r="T53" s="22"/>
       <c r="U53" s="36" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="W53" s="11" t="str">
         <f t="shared" si="0"/>
@@ -5160,7 +5160,7 @@
         <v>24</v>
       </c>
       <c r="F54" s="33" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="G54" s="14" t="s">
         <v>170</v>
@@ -5187,7 +5187,7 @@
         <v>112</v>
       </c>
       <c r="Q54" s="34" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="R54" s="16">
         <v>0.64583333333333337</v>
@@ -5197,7 +5197,7 @@
       </c>
       <c r="T54" s="22"/>
       <c r="U54" s="36" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="W54" s="11" t="str">
         <f t="shared" si="0"/>
@@ -5223,7 +5223,7 @@
         <v>39</v>
       </c>
       <c r="F55" s="33" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="G55" s="14" t="s">
         <v>174</v>
@@ -5250,7 +5250,7 @@
         <v>71</v>
       </c>
       <c r="Q55" s="34" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="R55" s="16">
         <v>0.67708333333333337</v>
@@ -5259,7 +5259,7 @@
         <v>31</v>
       </c>
       <c r="U55" s="35" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="W55" s="11" t="str">
         <f t="shared" si="0"/>
@@ -5285,7 +5285,7 @@
         <v>24</v>
       </c>
       <c r="F56" s="33" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="G56" s="14" t="s">
         <v>177</v>
@@ -5312,7 +5312,7 @@
         <v>71</v>
       </c>
       <c r="Q56" s="34" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="R56" s="16">
         <v>0.67708333333333337</v>
@@ -5321,7 +5321,7 @@
         <v>31</v>
       </c>
       <c r="U56" s="35" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="W56" s="11" t="str">
         <f t="shared" si="0"/>
@@ -5347,7 +5347,7 @@
         <v>39</v>
       </c>
       <c r="F57" s="33" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="G57" s="14" t="s">
         <v>180</v>
@@ -5374,7 +5374,7 @@
         <v>37</v>
       </c>
       <c r="Q57" s="34" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="R57" s="16">
         <v>0.67708333333333337</v>
@@ -5383,7 +5383,7 @@
         <v>31</v>
       </c>
       <c r="U57" s="35" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="W57" s="11" t="str">
         <f t="shared" si="0"/>
@@ -5409,7 +5409,7 @@
         <v>24</v>
       </c>
       <c r="F58" s="33" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="G58" s="14" t="s">
         <v>183</v>
@@ -5436,7 +5436,7 @@
         <v>37</v>
       </c>
       <c r="Q58" s="34" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="R58" s="16">
         <v>0.67708333333333337</v>
@@ -5445,7 +5445,7 @@
         <v>31</v>
       </c>
       <c r="U58" s="35" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="W58" s="11" t="str">
         <f t="shared" si="0"/>
@@ -5471,7 +5471,7 @@
         <v>39</v>
       </c>
       <c r="F59" s="33" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="G59" s="14" t="s">
         <v>186</v>
@@ -5498,7 +5498,7 @@
         <v>37</v>
       </c>
       <c r="Q59" s="34" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="R59" s="16">
         <v>0.67708333333333337</v>
@@ -5507,7 +5507,7 @@
         <v>31</v>
       </c>
       <c r="U59" s="35" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="W59" s="11" t="str">
         <f t="shared" si="0"/>
@@ -5533,7 +5533,7 @@
         <v>24</v>
       </c>
       <c r="F60" s="33" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="G60" s="14" t="s">
         <v>189</v>
@@ -5560,7 +5560,7 @@
         <v>59</v>
       </c>
       <c r="Q60" s="34" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="R60" s="16">
         <v>0.66666666666666663</v>
@@ -5569,7 +5569,7 @@
         <v>31</v>
       </c>
       <c r="U60" s="35" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="W60" s="11" t="str">
         <f t="shared" si="0"/>
@@ -5589,21 +5589,21 @@
         <v>42569</v>
       </c>
       <c r="D61" s="11" t="s">
-        <v>192</v>
+        <v>432</v>
       </c>
       <c r="E61" s="11" t="s">
         <v>39</v>
       </c>
       <c r="F61" s="33" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="G61" s="14" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="H61" s="14"/>
       <c r="I61" s="14"/>
       <c r="J61" s="14" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="K61" s="14"/>
       <c r="L61" s="11" t="s">
@@ -5622,7 +5622,7 @@
         <v>104</v>
       </c>
       <c r="Q61" s="34" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="R61" s="16">
         <v>0.66666666666666663</v>
@@ -5631,7 +5631,7 @@
         <v>31</v>
       </c>
       <c r="U61" s="35" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="W61" s="11" t="str">
         <f t="shared" si="0"/>
@@ -5645,27 +5645,27 @@
     <row r="62" spans="1:24" s="11" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A62" s="10"/>
       <c r="B62" s="11" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C62" s="12">
         <v>42569</v>
       </c>
       <c r="D62" s="11" t="s">
-        <v>192</v>
+        <v>432</v>
       </c>
       <c r="E62" s="11" t="s">
         <v>24</v>
       </c>
       <c r="F62" s="33" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="G62" s="14" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="H62" s="14"/>
       <c r="I62" s="14"/>
       <c r="J62" s="14" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="K62" s="14"/>
       <c r="L62" s="11" t="s">
@@ -5684,7 +5684,7 @@
         <v>104</v>
       </c>
       <c r="Q62" s="34" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="R62" s="16">
         <v>0.66666666666666663</v>
@@ -5693,7 +5693,7 @@
         <v>31</v>
       </c>
       <c r="U62" s="35" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="W62" s="11" t="str">
         <f t="shared" si="0"/>
@@ -5707,27 +5707,27 @@
     <row r="63" spans="1:24" s="11" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A63" s="10"/>
       <c r="B63" s="11" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C63" s="12">
         <v>42569</v>
       </c>
       <c r="D63" s="11" t="s">
-        <v>192</v>
+        <v>432</v>
       </c>
       <c r="E63" s="11" t="s">
         <v>39</v>
       </c>
       <c r="F63" s="33" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="G63" s="14" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="H63" s="14"/>
       <c r="I63" s="14"/>
       <c r="J63" s="14" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="K63" s="14"/>
       <c r="L63" s="11" t="s">
@@ -5746,7 +5746,7 @@
         <v>104</v>
       </c>
       <c r="Q63" s="34" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="R63" s="16">
         <v>0.66666666666666663</v>
@@ -5756,7 +5756,7 @@
       </c>
       <c r="T63" s="22"/>
       <c r="U63" s="36" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="W63" s="11" t="str">
         <f t="shared" si="0"/>
@@ -5770,7 +5770,7 @@
     <row r="64" spans="1:24" s="11" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A64" s="10"/>
       <c r="B64" s="11" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C64" s="12">
         <v>42569</v>
@@ -5782,15 +5782,15 @@
         <v>24</v>
       </c>
       <c r="F64" s="33" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="G64" s="14" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="H64" s="14"/>
       <c r="I64" s="14"/>
       <c r="J64" s="14" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="K64" s="14"/>
       <c r="L64" s="11" t="s">
@@ -5809,7 +5809,7 @@
         <v>23</v>
       </c>
       <c r="Q64" s="34" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="R64" s="16">
         <v>0.6875</v>
@@ -5818,7 +5818,7 @@
         <v>31</v>
       </c>
       <c r="U64" s="35" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="W64" s="11" t="str">
         <f t="shared" si="0"/>
@@ -5832,7 +5832,7 @@
     <row r="65" spans="1:24" s="11" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A65" s="10"/>
       <c r="B65" s="11" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C65" s="12">
         <v>42569</v>
@@ -5844,15 +5844,15 @@
         <v>39</v>
       </c>
       <c r="F65" s="33" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="G65" s="14" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="H65" s="14"/>
       <c r="I65" s="14"/>
       <c r="J65" s="14" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="K65" s="14"/>
       <c r="L65" s="11" t="s">
@@ -5871,7 +5871,7 @@
         <v>112</v>
       </c>
       <c r="Q65" s="34" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="R65" s="16">
         <v>0.6875</v>
@@ -5880,7 +5880,7 @@
         <v>31</v>
       </c>
       <c r="U65" s="35" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="W65" s="11" t="str">
         <f t="shared" si="0"/>
@@ -5894,7 +5894,7 @@
     <row r="66" spans="1:24" s="11" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A66" s="10"/>
       <c r="B66" s="11" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C66" s="12">
         <v>42569</v>
@@ -5906,15 +5906,15 @@
         <v>39</v>
       </c>
       <c r="F66" s="33" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="G66" s="14" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="H66" s="14"/>
       <c r="I66" s="14"/>
       <c r="J66" s="14" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="K66" s="14"/>
       <c r="L66" s="11" t="s">
@@ -5933,7 +5933,7 @@
         <v>112</v>
       </c>
       <c r="Q66" s="34" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="R66" s="16">
         <v>0.6875</v>
@@ -5942,7 +5942,7 @@
         <v>31</v>
       </c>
       <c r="U66" s="35" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="W66" s="11" t="str">
         <f t="shared" si="0"/>
@@ -5956,7 +5956,7 @@
     <row r="67" spans="1:24" s="11" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A67" s="10"/>
       <c r="B67" s="11" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C67" s="12">
         <v>42569</v>
@@ -5968,15 +5968,15 @@
         <v>24</v>
       </c>
       <c r="F67" s="33" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="G67" s="14" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="H67" s="14"/>
       <c r="I67" s="14"/>
       <c r="J67" s="14" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="K67" s="14"/>
       <c r="L67" s="11" t="s">
@@ -5995,7 +5995,7 @@
         <v>112</v>
       </c>
       <c r="Q67" s="34" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="R67" s="16">
         <v>0.6875</v>
@@ -6004,7 +6004,7 @@
         <v>31</v>
       </c>
       <c r="U67" s="35" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="W67" s="11" t="str">
         <f t="shared" si="0"/>
@@ -6018,7 +6018,7 @@
     <row r="68" spans="1:24" s="11" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A68" s="10"/>
       <c r="B68" s="11" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C68" s="12">
         <v>42569</v>
@@ -6030,7 +6030,7 @@
         <v>39</v>
       </c>
       <c r="F68" s="33" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="G68" s="14"/>
       <c r="H68" s="14"/>
@@ -6053,7 +6053,7 @@
         <v>112</v>
       </c>
       <c r="Q68" s="34" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="R68" s="16">
         <v>0.6875</v>
@@ -6062,7 +6062,7 @@
         <v>31</v>
       </c>
       <c r="U68" s="35" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="W68" s="11" t="str">
         <f t="shared" ref="W68:W131" si="1">CONCATENATE(L68,M68,N68,O68,Q68)</f>
@@ -6076,7 +6076,7 @@
     <row r="69" spans="1:24" s="11" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A69" s="10"/>
       <c r="B69" s="11" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C69" s="12">
         <v>42569</v>
@@ -6088,15 +6088,15 @@
         <v>39</v>
       </c>
       <c r="F69" s="33" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="G69" s="14" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="H69" s="14"/>
       <c r="I69" s="14"/>
       <c r="J69" s="14" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="K69" s="14"/>
       <c r="L69" s="11" t="s">
@@ -6106,7 +6106,7 @@
         <v>28</v>
       </c>
       <c r="N69" s="11" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="O69" s="11" t="s">
         <v>30</v>
@@ -6115,7 +6115,7 @@
         <v>23</v>
       </c>
       <c r="Q69" s="34" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="R69" s="16">
         <v>0.70833333333333337</v>
@@ -6124,7 +6124,7 @@
         <v>31</v>
       </c>
       <c r="U69" s="35" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="W69" s="11" t="str">
         <f t="shared" si="1"/>
@@ -6138,7 +6138,7 @@
     <row r="70" spans="1:24" s="11" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A70" s="10"/>
       <c r="B70" s="11" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C70" s="12">
         <v>42569</v>
@@ -6150,15 +6150,15 @@
         <v>24</v>
       </c>
       <c r="F70" s="33" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="G70" s="14" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="H70" s="14"/>
       <c r="I70" s="14"/>
       <c r="J70" s="14" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="K70" s="14"/>
       <c r="L70" s="11" t="s">
@@ -6168,7 +6168,7 @@
         <v>28</v>
       </c>
       <c r="N70" s="11" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="O70" s="11" t="s">
         <v>30</v>
@@ -6177,7 +6177,7 @@
         <v>23</v>
       </c>
       <c r="Q70" s="34" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="R70" s="16">
         <v>0.70833333333333337</v>
@@ -6186,7 +6186,7 @@
         <v>31</v>
       </c>
       <c r="U70" s="35" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="W70" s="11" t="str">
         <f t="shared" si="1"/>
@@ -6200,7 +6200,7 @@
     <row r="71" spans="1:24" s="11" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A71" s="10"/>
       <c r="B71" s="11" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C71" s="12">
         <v>42569</v>
@@ -6212,15 +6212,15 @@
         <v>39</v>
       </c>
       <c r="F71" s="33" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="G71" s="14" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="H71" s="14"/>
       <c r="I71" s="14"/>
       <c r="J71" s="14" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="K71" s="14"/>
       <c r="L71" s="11" t="s">
@@ -6230,7 +6230,7 @@
         <v>28</v>
       </c>
       <c r="N71" s="11" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="O71" s="11" t="s">
         <v>30</v>
@@ -6239,7 +6239,7 @@
         <v>112</v>
       </c>
       <c r="Q71" s="34" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="R71" s="16">
         <v>0.70833333333333337</v>
@@ -6248,7 +6248,7 @@
         <v>31</v>
       </c>
       <c r="U71" s="35" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="W71" s="11" t="str">
         <f t="shared" si="1"/>
@@ -6262,7 +6262,7 @@
     <row r="72" spans="1:24" s="11" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A72" s="10"/>
       <c r="B72" s="11" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C72" s="12">
         <v>42569</v>
@@ -6274,15 +6274,15 @@
         <v>39</v>
       </c>
       <c r="F72" s="33" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="G72" s="14" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="H72" s="14"/>
       <c r="I72" s="14"/>
       <c r="J72" s="14" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="K72" s="14"/>
       <c r="L72" s="11" t="s">
@@ -6301,7 +6301,7 @@
         <v>71</v>
       </c>
       <c r="Q72" s="34" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="R72" s="16">
         <v>0.70833333333333337</v>
@@ -6311,7 +6311,7 @@
       </c>
       <c r="T72" s="22"/>
       <c r="U72" s="36" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="W72" s="11" t="str">
         <f t="shared" si="1"/>
@@ -6325,7 +6325,7 @@
     <row r="73" spans="1:24" s="11" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A73" s="10"/>
       <c r="B73" s="11" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C73" s="12">
         <v>42569</v>
@@ -6337,15 +6337,15 @@
         <v>24</v>
       </c>
       <c r="F73" s="33" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="G73" s="14" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="H73" s="14"/>
       <c r="I73" s="14"/>
       <c r="J73" s="14" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="K73" s="14"/>
       <c r="L73" s="11" t="s">
@@ -6364,7 +6364,7 @@
         <v>71</v>
       </c>
       <c r="Q73" s="34" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="R73" s="16">
         <v>0.70833333333333337</v>
@@ -6374,7 +6374,7 @@
       </c>
       <c r="T73" s="22"/>
       <c r="U73" s="36" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="W73" s="11" t="str">
         <f t="shared" si="1"/>
@@ -6388,7 +6388,7 @@
     <row r="74" spans="1:24" s="11" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A74" s="10"/>
       <c r="B74" s="11" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C74" s="12">
         <v>42569</v>
@@ -6400,15 +6400,15 @@
         <v>24</v>
       </c>
       <c r="F74" s="33" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="G74" s="14" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="H74" s="14"/>
       <c r="I74" s="14"/>
       <c r="J74" s="14" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="K74" s="14"/>
       <c r="L74" s="11" t="s">
@@ -6427,7 +6427,7 @@
         <v>37</v>
       </c>
       <c r="Q74" s="34" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="R74" s="16">
         <v>0.70833333333333337</v>
@@ -6437,7 +6437,7 @@
       </c>
       <c r="T74" s="22"/>
       <c r="U74" s="36" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="W74" s="11" t="str">
         <f t="shared" si="1"/>
@@ -6451,7 +6451,7 @@
     <row r="75" spans="1:24" s="11" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A75" s="10"/>
       <c r="B75" s="14" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C75" s="12">
         <v>42569</v>
@@ -6463,15 +6463,15 @@
         <v>24</v>
       </c>
       <c r="F75" s="33" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="G75" s="14" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="H75" s="14"/>
       <c r="I75" s="14"/>
       <c r="J75" s="14" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="K75" s="14"/>
       <c r="L75" s="11" t="s">
@@ -6490,7 +6490,7 @@
         <v>37</v>
       </c>
       <c r="Q75" s="34" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="R75" s="16">
         <v>0.70833333333333337</v>
@@ -6499,7 +6499,7 @@
         <v>31</v>
       </c>
       <c r="U75" s="35" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="W75" s="11" t="str">
         <f t="shared" si="1"/>
@@ -6525,7 +6525,7 @@
         <v>39</v>
       </c>
       <c r="F76" s="33" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="G76" s="14" t="s">
         <v>77</v>
@@ -6552,7 +6552,7 @@
         <v>37</v>
       </c>
       <c r="Q76" s="34" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="R76" s="16">
         <v>0.70833333333333337</v>
@@ -6561,7 +6561,7 @@
         <v>31</v>
       </c>
       <c r="U76" s="35" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="W76" s="11" t="str">
         <f t="shared" si="1"/>
@@ -6575,7 +6575,7 @@
     <row r="77" spans="1:24" s="11" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A77" s="10"/>
       <c r="B77" s="11" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C77" s="12">
         <v>42569</v>
@@ -6587,15 +6587,15 @@
         <v>24</v>
       </c>
       <c r="F77" s="33" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="G77" s="14" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="H77" s="14"/>
       <c r="I77" s="14"/>
       <c r="J77" s="14" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="K77" s="14"/>
       <c r="L77" s="11" t="s">
@@ -6614,7 +6614,7 @@
         <v>80</v>
       </c>
       <c r="Q77" s="34" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="R77" s="16">
         <v>0.70833333333333337</v>
@@ -6623,7 +6623,7 @@
         <v>31</v>
       </c>
       <c r="U77" s="35" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="W77" s="11" t="str">
         <f t="shared" si="1"/>
@@ -6637,7 +6637,7 @@
     <row r="78" spans="1:24" s="11" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A78" s="10"/>
       <c r="B78" s="11" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C78" s="12">
         <v>42569</v>
@@ -6649,15 +6649,15 @@
         <v>39</v>
       </c>
       <c r="F78" s="33" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="G78" s="14" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="H78" s="14"/>
       <c r="I78" s="14"/>
       <c r="J78" s="14" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="K78" s="21"/>
       <c r="L78" s="11" t="s">
@@ -6676,7 +6676,7 @@
         <v>80</v>
       </c>
       <c r="Q78" s="34" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="R78" s="16">
         <v>0.70833333333333337</v>
@@ -6685,7 +6685,7 @@
         <v>31</v>
       </c>
       <c r="U78" s="35" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="W78" s="11" t="str">
         <f t="shared" si="1"/>
@@ -6699,7 +6699,7 @@
     <row r="79" spans="1:24" s="11" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A79" s="10"/>
       <c r="B79" s="11" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C79" s="12">
         <v>42569</v>
@@ -6711,15 +6711,15 @@
         <v>24</v>
       </c>
       <c r="F79" s="33" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="G79" s="14" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="H79" s="14"/>
       <c r="I79" s="14"/>
       <c r="J79" s="14" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="K79" s="21"/>
       <c r="L79" s="11" t="s">
@@ -6738,7 +6738,7 @@
         <v>47</v>
       </c>
       <c r="Q79" s="34" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="R79" s="16">
         <v>0.70833333333333337</v>
@@ -6747,7 +6747,7 @@
         <v>31</v>
       </c>
       <c r="U79" s="35" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="W79" s="11" t="str">
         <f t="shared" si="1"/>
@@ -6761,7 +6761,7 @@
     <row r="80" spans="1:24" s="11" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A80" s="10"/>
       <c r="B80" s="11" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C80" s="12">
         <v>42569</v>
@@ -6773,15 +6773,15 @@
         <v>24</v>
       </c>
       <c r="F80" s="33" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="G80" s="14" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="H80" s="14"/>
       <c r="I80" s="14"/>
       <c r="J80" s="14" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="K80" s="21"/>
       <c r="L80" s="11" t="s">
@@ -6800,7 +6800,7 @@
         <v>47</v>
       </c>
       <c r="Q80" s="34" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="R80" s="16">
         <v>0.70833333333333337</v>
@@ -6809,7 +6809,7 @@
         <v>31</v>
       </c>
       <c r="U80" s="35" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="W80" s="11" t="str">
         <f t="shared" si="1"/>
@@ -6823,7 +6823,7 @@
     <row r="81" spans="1:24" s="11" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A81" s="10"/>
       <c r="B81" s="11" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C81" s="12">
         <v>42569</v>
@@ -6835,15 +6835,15 @@
         <v>24</v>
       </c>
       <c r="F81" s="33" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="G81" s="14" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="H81" s="14"/>
       <c r="I81" s="14"/>
       <c r="J81" s="14" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="K81" s="18"/>
       <c r="L81" s="11" t="s">
@@ -6862,7 +6862,7 @@
         <v>47</v>
       </c>
       <c r="Q81" s="34" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="R81" s="16">
         <v>0.70833333333333337</v>
@@ -6871,7 +6871,7 @@
         <v>31</v>
       </c>
       <c r="U81" s="35" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="W81" s="11" t="str">
         <f t="shared" si="1"/>
@@ -6885,27 +6885,27 @@
     <row r="82" spans="1:24" s="11" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A82" s="10"/>
       <c r="B82" s="11" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C82" s="12">
         <v>42569</v>
       </c>
       <c r="D82" s="11" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E82" s="11" t="s">
         <v>24</v>
       </c>
       <c r="F82" s="33" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="G82" s="14" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="H82" s="14"/>
       <c r="I82" s="14"/>
       <c r="J82" s="14" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="K82" s="21"/>
       <c r="L82" s="11" t="s">
@@ -6924,7 +6924,7 @@
         <v>59</v>
       </c>
       <c r="Q82" s="34" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="R82" s="16">
         <v>0.625</v>
@@ -6933,7 +6933,7 @@
         <v>31</v>
       </c>
       <c r="U82" s="35" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="W82" s="11" t="str">
         <f t="shared" si="1"/>
@@ -6947,7 +6947,7 @@
     <row r="83" spans="1:24" s="11" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A83" s="10"/>
       <c r="B83" s="11" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C83" s="12">
         <v>42569</v>
@@ -6959,15 +6959,15 @@
         <v>39</v>
       </c>
       <c r="F83" s="33" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="G83" s="14" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="H83" s="14"/>
       <c r="I83" s="14"/>
       <c r="J83" s="14" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="K83" s="14"/>
       <c r="L83" s="11" t="s">
@@ -6986,7 +6986,7 @@
         <v>59</v>
       </c>
       <c r="Q83" s="34" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="R83" s="16">
         <v>0.625</v>
@@ -6995,7 +6995,7 @@
         <v>31</v>
       </c>
       <c r="U83" s="35" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="W83" s="11" t="str">
         <f t="shared" si="1"/>
@@ -7009,7 +7009,7 @@
     <row r="84" spans="1:24" s="11" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A84" s="10"/>
       <c r="B84" s="11" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C84" s="12">
         <v>42569</v>
@@ -7021,15 +7021,15 @@
         <v>24</v>
       </c>
       <c r="F84" s="33" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="G84" s="14" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="H84" s="14"/>
       <c r="I84" s="14"/>
       <c r="J84" s="14" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="K84" s="14"/>
       <c r="L84" s="11" t="s">
@@ -7048,7 +7048,7 @@
         <v>59</v>
       </c>
       <c r="Q84" s="34" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="R84" s="16">
         <v>0.625</v>
@@ -7057,7 +7057,7 @@
         <v>31</v>
       </c>
       <c r="U84" s="35" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="W84" s="11" t="str">
         <f t="shared" si="1"/>
@@ -7071,7 +7071,7 @@
     <row r="85" spans="1:24" s="11" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A85" s="10"/>
       <c r="B85" s="11" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C85" s="12">
         <v>42569</v>
@@ -7083,15 +7083,15 @@
         <v>24</v>
       </c>
       <c r="F85" s="33" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="G85" s="14" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="H85" s="14"/>
       <c r="I85" s="14"/>
       <c r="J85" s="14" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="K85" s="14"/>
       <c r="L85" s="11" t="s">
@@ -7110,7 +7110,7 @@
         <v>59</v>
       </c>
       <c r="Q85" s="34" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="R85" s="16">
         <v>0.625</v>
@@ -7119,7 +7119,7 @@
         <v>31</v>
       </c>
       <c r="U85" s="35" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="W85" s="11" t="str">
         <f t="shared" si="1"/>
@@ -7133,7 +7133,7 @@
     <row r="86" spans="1:24" s="11" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A86" s="10"/>
       <c r="B86" s="11" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C86" s="12">
         <v>42569</v>
@@ -7145,15 +7145,15 @@
         <v>39</v>
       </c>
       <c r="F86" s="33" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="G86" s="14" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="H86" s="14"/>
       <c r="I86" s="14"/>
       <c r="J86" s="14" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="K86" s="21"/>
       <c r="L86" s="11" t="s">
@@ -7172,7 +7172,7 @@
         <v>59</v>
       </c>
       <c r="Q86" s="34" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="R86" s="16">
         <v>0.625</v>
@@ -7181,7 +7181,7 @@
         <v>31</v>
       </c>
       <c r="U86" s="35" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="W86" s="11" t="str">
         <f t="shared" si="1"/>
@@ -7195,7 +7195,7 @@
     <row r="87" spans="1:24" s="11" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A87" s="10"/>
       <c r="B87" s="11" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C87" s="12">
         <v>42569</v>
@@ -7204,15 +7204,15 @@
         <v>57</v>
       </c>
       <c r="F87" s="33" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="G87" s="14" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="H87" s="14"/>
       <c r="I87" s="14"/>
       <c r="J87" s="14" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="K87" s="14"/>
       <c r="L87" s="11" t="s">
@@ -7231,7 +7231,7 @@
         <v>59</v>
       </c>
       <c r="Q87" s="34" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="R87" s="16">
         <v>0.625</v>
@@ -7241,7 +7241,7 @@
       </c>
       <c r="T87" s="22"/>
       <c r="U87" s="36" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="W87" s="11" t="str">
         <f t="shared" si="1"/>
@@ -7255,7 +7255,7 @@
     <row r="88" spans="1:24" s="11" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A88" s="10"/>
       <c r="B88" s="11" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C88" s="12">
         <v>42569</v>
@@ -7267,15 +7267,15 @@
         <v>39</v>
       </c>
       <c r="F88" s="33" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="G88" s="14" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="H88" s="14"/>
       <c r="I88" s="14"/>
       <c r="J88" s="14" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="K88" s="14"/>
       <c r="L88" s="11" t="s">
@@ -7294,7 +7294,7 @@
         <v>59</v>
       </c>
       <c r="Q88" s="34" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="R88" s="16">
         <v>0.625</v>
@@ -7304,7 +7304,7 @@
       </c>
       <c r="T88" s="22"/>
       <c r="U88" s="36" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="W88" s="11" t="str">
         <f t="shared" si="1"/>
@@ -7318,7 +7318,7 @@
     <row r="89" spans="1:24" s="11" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A89" s="10"/>
       <c r="B89" s="11" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C89" s="12">
         <v>42569</v>
@@ -7330,15 +7330,15 @@
         <v>39</v>
       </c>
       <c r="F89" s="33" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="G89" s="14" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="H89" s="14"/>
       <c r="I89" s="14"/>
       <c r="J89" s="14" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="K89" s="14"/>
       <c r="L89" s="11" t="s">
@@ -7357,7 +7357,7 @@
         <v>59</v>
       </c>
       <c r="Q89" s="34" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="R89" s="16">
         <v>0.625</v>
@@ -7367,7 +7367,7 @@
       </c>
       <c r="T89" s="22"/>
       <c r="U89" s="36" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="W89" s="11" t="str">
         <f t="shared" si="1"/>
@@ -7381,7 +7381,7 @@
     <row r="90" spans="1:24" s="11" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A90" s="10"/>
       <c r="B90" s="11" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C90" s="12">
         <v>42569</v>
@@ -7393,15 +7393,15 @@
         <v>24</v>
       </c>
       <c r="F90" s="33" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="G90" s="14" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="H90" s="14"/>
       <c r="I90" s="14"/>
       <c r="J90" s="14" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="K90" s="21"/>
       <c r="L90" s="11" t="s">
@@ -7420,7 +7420,7 @@
         <v>69</v>
       </c>
       <c r="Q90" s="34" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="R90" s="16">
         <v>0.625</v>
@@ -7430,7 +7430,7 @@
       </c>
       <c r="T90" s="22"/>
       <c r="U90" s="36" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="W90" s="11" t="str">
         <f t="shared" si="1"/>
@@ -7444,27 +7444,27 @@
     <row r="91" spans="1:24" s="11" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A91" s="10"/>
       <c r="B91" s="11" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C91" s="12">
         <v>42569</v>
       </c>
       <c r="D91" s="11" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="E91" s="11" t="s">
         <v>24</v>
       </c>
       <c r="F91" s="33" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="G91" s="14" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="H91" s="14"/>
       <c r="I91" s="14"/>
       <c r="J91" s="14" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="K91" s="14"/>
       <c r="L91" s="11" t="s">
@@ -7483,7 +7483,7 @@
         <v>69</v>
       </c>
       <c r="Q91" s="34" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="R91" s="16">
         <v>0.625</v>
@@ -7493,7 +7493,7 @@
       </c>
       <c r="T91" s="22"/>
       <c r="U91" s="36" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="W91" s="11" t="str">
         <f t="shared" si="1"/>
@@ -7507,27 +7507,27 @@
     <row r="92" spans="1:24" s="11" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A92" s="10"/>
       <c r="B92" s="11" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C92" s="12">
         <v>42569</v>
       </c>
       <c r="D92" s="11" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="E92" s="11" t="s">
         <v>39</v>
       </c>
       <c r="F92" s="33" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="G92" s="14" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="H92" s="14"/>
       <c r="I92" s="14"/>
       <c r="J92" s="14" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="K92" s="18"/>
       <c r="L92" s="11" t="s">
@@ -7546,7 +7546,7 @@
         <v>69</v>
       </c>
       <c r="Q92" s="34" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="R92" s="16">
         <v>0.625</v>
@@ -7556,7 +7556,7 @@
       </c>
       <c r="T92" s="22"/>
       <c r="U92" s="36" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="W92" s="11" t="str">
         <f t="shared" si="1"/>
@@ -7570,7 +7570,7 @@
     <row r="93" spans="1:24" s="11" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A93" s="10"/>
       <c r="B93" s="11" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C93" s="12">
         <v>42569</v>
@@ -7582,15 +7582,15 @@
         <v>24</v>
       </c>
       <c r="F93" s="33" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="G93" s="14" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="H93" s="14"/>
       <c r="I93" s="14"/>
       <c r="J93" s="14" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="K93" s="14"/>
       <c r="L93" s="11" t="s">
@@ -7609,7 +7609,7 @@
         <v>69</v>
       </c>
       <c r="Q93" s="34" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="R93" s="16">
         <v>0.625</v>
@@ -7619,7 +7619,7 @@
       </c>
       <c r="T93" s="22"/>
       <c r="U93" s="36" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="W93" s="11" t="str">
         <f t="shared" si="1"/>

</xml_diff>